<commit_message>
no shuffle, scale wind speeds as well, arrange benchmarks
</commit_message>
<xml_diff>
--- a/Hyperparameter_Search.xlsx
+++ b/Hyperparameter_Search.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca0e08f364b50fd3/Dokumente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Webapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AAA2BC0-89E1-4BAE-9F72-0EA98318BA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2F14F9-53AA-443E-ADE3-569A32DE21AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{71890C88-FA0A-4DE6-B057-18D13399F0CF}"/>
+    <workbookView xWindow="0" yWindow="270" windowWidth="23980" windowHeight="15010" xr2:uid="{71890C88-FA0A-4DE6-B057-18D13399F0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>hidden_size</t>
   </si>
@@ -53,9 +54,6 @@
     <t>number_folds</t>
   </si>
   <si>
-    <t>HuberLoss 1st fold</t>
-  </si>
-  <si>
     <t>the higher, the better, barely increases computational time</t>
   </si>
   <si>
@@ -80,13 +78,37 @@
     <t>4 Linear, 3 ReLU in between, sizes 256-128-64</t>
   </si>
   <si>
-    <t>4 Linear, 3 Batch Normalisaiton, ReLU, Dropout  in between, sizes 256-128-64</t>
-  </si>
-  <si>
-    <t>3 Linear, 2 Batch Normalisaiton, ReLU, Dropout  in between, sizes 256-64</t>
-  </si>
-  <si>
     <t>5 Linear, 4 ReLU in between, sizes 256-128-64-32</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>Huber</t>
+  </si>
+  <si>
+    <t>MAE / MW</t>
+  </si>
+  <si>
+    <t>MSE /MW²</t>
+  </si>
+  <si>
+    <t>4 Linear, 3 LeakyReLU in between, sizes 256-128-64</t>
+  </si>
+  <si>
+    <t>HuberLoss 1st fold, test 2</t>
+  </si>
+  <si>
+    <t>HuberLoss 1st fold, test 1</t>
+  </si>
+  <si>
+    <t>4 Linear, 3 Batch Normalisaton, ReLU, Dropout  in between, sizes 256-128-64</t>
+  </si>
+  <si>
+    <t>3 Linear, 2 Batch Normalisaton, ReLU, Dropout  in between, sizes 256-64</t>
+  </si>
+  <si>
+    <t>5 Linear, 4 LeakyReLU in between, sizes 256-128-64-32</t>
   </si>
 </sst>
 </file>
@@ -102,12 +124,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,9 +150,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,6 +170,36 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5DF4185-7D09-482C-B551-D12CDF735AD0}" name="Table2" displayName="Table2" ref="A1:H24" totalsRowShown="0">
+  <autoFilter ref="A1:H24" xr:uid="{E5DF4185-7D09-482C-B551-D12CDF735AD0}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{DC54D89C-B187-470B-A73E-9595AC905D54}" name="hidden_size"/>
+    <tableColumn id="2" xr3:uid="{4865C0F4-76F1-4F26-A024-57E1FB83BD98}" name="batch_size"/>
+    <tableColumn id="3" xr3:uid="{925130B2-7BA6-4EB7-954B-6B6B681EAB57}" name="learning_rate"/>
+    <tableColumn id="4" xr3:uid="{7FB3056B-662B-4219-A011-4DD16738369E}" name="number_epochs"/>
+    <tableColumn id="5" xr3:uid="{A80783D7-789E-4508-85BD-76CD8DF2B057}" name="number_folds"/>
+    <tableColumn id="6" xr3:uid="{05C7F77A-35FC-4154-B856-7B5788BECF81}" name="configuration"/>
+    <tableColumn id="7" xr3:uid="{20D64F6D-6607-4B45-8B4E-114BF90DEACE}" name="HuberLoss 1st fold, test 1"/>
+    <tableColumn id="8" xr3:uid="{7A22A143-39AD-432A-A231-3D5CE186C3F6}" name="HuberLoss 1st fold, test 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BF0D451-C4EC-4C76-9533-946C338A61F1}" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{9BF0D451-C4EC-4C76-9533-946C338A61F1}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D6A26C0A-B170-414A-9726-CCF11976421E}" name="Benchmark"/>
+    <tableColumn id="2" xr3:uid="{015C6591-6245-40B5-BB2D-76513559F01D}" name="Huber"/>
+    <tableColumn id="3" xr3:uid="{2A4C1E94-F15F-48EB-9380-5F928EB498CE}" name="MAE / MW"/>
+    <tableColumn id="4" xr3:uid="{320F445D-AC0A-4F8E-B04F-0E25183BD0DB}" name="MSE /MW²"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,15 +519,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B619DEB1-2169-4C96-A144-21EC908D0785}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" customWidth="1"/>
+    <col min="6" max="6" width="62.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,13 +554,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4</v>
       </c>
@@ -507,13 +580,13 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>35.369999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>8</v>
       </c>
@@ -521,7 +594,7 @@
         <v>29.28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>16</v>
       </c>
@@ -529,7 +602,7 @@
         <v>27.01</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>32</v>
       </c>
@@ -537,7 +610,7 @@
         <v>24.75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>64</v>
       </c>
@@ -545,7 +618,7 @@
         <v>23.94</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>128</v>
       </c>
@@ -553,17 +626,17 @@
         <v>23.86</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>256</v>
       </c>
       <c r="G8">
         <v>23.24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>128</v>
@@ -572,7 +645,7 @@
         <v>23.85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>32</v>
       </c>
@@ -580,7 +653,7 @@
         <v>22.56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>16</v>
       </c>
@@ -588,7 +661,7 @@
         <v>20.98</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>8</v>
       </c>
@@ -596,26 +669,26 @@
         <v>20.39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="2">
         <v>4</v>
       </c>
       <c r="G13">
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3">
         <v>0.01</v>
       </c>
       <c r="G14">
         <v>19.57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15" s="1">
         <v>1E-4</v>
       </c>
@@ -623,7 +696,7 @@
         <v>24.63</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>32</v>
       </c>
@@ -634,61 +707,165 @@
         <v>1E-3</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16">
         <v>22.25</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:8" x14ac:dyDescent="0.35">
       <c r="F17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17">
         <v>37.64</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.35">
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18">
         <v>19.77</v>
       </c>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F19" t="s">
-        <v>13</v>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F19" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G19">
         <v>18.649999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.35">
       <c r="F20" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G20">
         <v>19.45</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:8" x14ac:dyDescent="0.35">
       <c r="F21" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G21">
         <v>19.27</v>
       </c>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:8" x14ac:dyDescent="0.35">
       <c r="F22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G22">
         <v>18.87</v>
       </c>
+      <c r="H22">
+        <v>18.43</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23">
+        <v>18.760000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>18.38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89C0B56-1B29-407E-B99F-D49EFD255F23}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>27.33</v>
+      </c>
+      <c r="C2">
+        <v>27.79</v>
+      </c>
+      <c r="D2">
+        <v>2986</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>25.53</v>
+      </c>
+      <c r="C3">
+        <v>25.99</v>
+      </c>
+      <c r="D3">
+        <v>2728.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>28.01</v>
+      </c>
+      <c r="C4">
+        <v>28.48</v>
+      </c>
+      <c r="D4">
+        <v>3127.33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bayesian Optimisation with optuna, shapley values
</commit_message>
<xml_diff>
--- a/Hyperparameter_Search.xlsx
+++ b/Hyperparameter_Search.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Webapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca0e08f364b50fd3/Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2F14F9-53AA-443E-ADE3-569A32DE21AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{4A76C159-DB73-4A01-8E62-CC878C9E5D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3949E84F-63E8-43C4-9453-04C10D091212}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="270" windowWidth="23980" windowHeight="15010" xr2:uid="{71890C88-FA0A-4DE6-B057-18D13399F0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{71890C88-FA0A-4DE6-B057-18D13399F0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>hidden_size</t>
   </si>
@@ -81,18 +81,6 @@
     <t>5 Linear, 4 ReLU in between, sizes 256-128-64-32</t>
   </si>
   <si>
-    <t>Benchmark</t>
-  </si>
-  <si>
-    <t>Huber</t>
-  </si>
-  <si>
-    <t>MAE / MW</t>
-  </si>
-  <si>
-    <t>MSE /MW²</t>
-  </si>
-  <si>
     <t>4 Linear, 3 LeakyReLU in between, sizes 256-128-64</t>
   </si>
   <si>
@@ -109,16 +97,201 @@
   </si>
   <si>
     <t>5 Linear, 4 LeakyReLU in between, sizes 256-128-64-32</t>
+  </si>
+  <si>
+    <t>HuberLoss 1st fold, test 3</t>
+  </si>
+  <si>
+    <t>subset of data</t>
+  </si>
+  <si>
+    <t>continuous</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>shuffle</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>7.6, 16.7</t>
+  </si>
+  <si>
+    <t>9.5, 9.5</t>
+  </si>
+  <si>
+    <t>training loss, validation loss</t>
+  </si>
+  <si>
+    <t>18.59, 18.74</t>
+  </si>
+  <si>
+    <t>18.55, 19.02</t>
+  </si>
+  <si>
+    <t>shuffle=True</t>
+  </si>
+  <si>
+    <t>shuffle = True</t>
+  </si>
+  <si>
+    <t>shuffle = False</t>
+  </si>
+  <si>
+    <t>subset of data=random</t>
+  </si>
+  <si>
+    <t>ordered</t>
+  </si>
+  <si>
+    <t>ordered on large scale (TimeSeriesSplit), random on small scale (DataLoader)</t>
+  </si>
+  <si>
+    <t>spatial (train test split)</t>
+  </si>
+  <si>
+    <t>random on large scale (K Fold Cross Validation with KFold), arbitrary on small scale (DataLoader)</t>
+  </si>
+  <si>
+    <t>ordered on large scale (K Fold Cross Validation with KFold), ordered on small scale (DataLoader)</t>
+  </si>
+  <si>
+    <t>10 first wpps</t>
+  </si>
+  <si>
+    <t>hidden_size=32</t>
+  </si>
+  <si>
+    <t>batch_size=32</t>
+  </si>
+  <si>
+    <t>lr=1e-3</t>
+  </si>
+  <si>
+    <t>number_epochs=20</t>
+  </si>
+  <si>
+    <t>n_splits=2</t>
+  </si>
+  <si>
+    <t>HuberLoss after 3 epochs of first fold, rounded without decimal places</t>
+  </si>
+  <si>
+    <t>ordered on large scale (TimeSeriesSplit), ordered on small scale (DataLoader)</t>
+  </si>
+  <si>
+    <t>order of data splitting</t>
+  </si>
+  <si>
+    <t>1. spatially</t>
+  </si>
+  <si>
+    <t>2. temporally</t>
+  </si>
+  <si>
+    <t>train_test_split on all data points with shuffle = False
+KFold with shuffle = False
+DataLoader with shuffle = False
+training loss = 9
+validation loss = 96
+temporal split of data is along the data chain and not as per indices as explained in PowerPoint diagram --&gt; train and validation dataset contain completely different wpps --&gt; signficant overfitting of the model to the wpps seen in the training data</t>
+  </si>
+  <si>
+    <t>Shuffling of data in mini batches by DataLoader is common, even for time series (?), to avoid overfitting and to get better gradients for more stable training</t>
+  </si>
+  <si>
+    <t>two written source code</t>
+  </si>
+  <si>
+    <t>temporal (cross fold validation, only for training and validation)</t>
+  </si>
+  <si>
+    <t>1. K Fold Cross Validation (train_test_split on all data points)</t>
+  </si>
+  <si>
+    <t>2. Time Series Cross Validation (train_test_split on wpps)</t>
+  </si>
+  <si>
+    <t>The TimeSeriesSplit method not only yields the better results, but also permits evaluation of the model's capability to generalise for new times and wpps, that it hasn't encountered previously.</t>
+  </si>
+  <si>
+    <t>train_test_split on wpps with shuffle = False
+TimeSeriesSplit
+DataLoader with shuffle = False
+training loss = 32; 36; 35; 33
+validation loss = 40; 52; 47; 35
+small overfitting compared to version where DataLoader shuffles, see PowerPoint diagram</t>
+  </si>
+  <si>
+    <t>train_test_split on wpps with shuffle = False
+TimeSeriesSplit
+DataLoader with shuffle = True
+training loss = 17; 17; 17
+validation loss = 16; 21; 18
+considering temporal structure, but shuffling in DataLoader to prevent overfitting, see PowerPoint diagram</t>
+  </si>
+  <si>
+    <t>train_test_split on wpps with shuffle = True
+TimeSeriesSplit
+DataLoader with shuffle = True
+training loss = 9; 17; 16; 17
+validation loss = 9; 16; 17; 17
+considering temporal structure, but shuffling in DataLoader to prevent overfitting</t>
+  </si>
+  <si>
+    <t>train_test_split on wpps with shuffle = True
+TimeSeriesSplit
+DataLoader with shuffle = False
+training loss = 8; 37; 32
+validation loss = 11; 68; 25
+small overfitting compared to version where DataLoader shuffles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">train_test_split on all data points with shuffle = False
+KFold with shuffle = True
+DataLoader with shuffle = arbitrary
+training loss = 17; 18; 17
+validation loss = 19; 20; 20
+shuffling only in the training+validation subset than globally is worse, when the temporal structure is not maintained anyway, because then the arbitrary patterns the model learns are overfitted to the wpps in the training and validation data compared to the testing data
+</t>
+  </si>
+  <si>
+    <t>train_test_split on all data points with shuffle = True
+KFold with shuffle = arbitrary
+DataLoader with shuffle = arbitrary
+training loss = 14; 15; 15
+validation loss = 14; 16; 15
+model learns arbitrary patterns in the entirety of the dataset, same as below</t>
+  </si>
+  <si>
+    <t>train_test_split on all data points with shuffle = True
+KFold with shuffle = arbitrary
+DataLoader with shuffle = arbitrary
+training loss = 14; 15; 15
+validation loss = 14; 16; 15
+model learns arbitrary patterns in the entirety of the dataset, same as above</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,11 +323,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,9 +355,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5DF4185-7D09-482C-B551-D12CDF735AD0}" name="Table2" displayName="Table2" ref="A1:H24" totalsRowShown="0">
-  <autoFilter ref="A1:H24" xr:uid="{E5DF4185-7D09-482C-B551-D12CDF735AD0}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5DF4185-7D09-482C-B551-D12CDF735AD0}" name="Table2" displayName="Table2" ref="A1:I24" totalsRowShown="0">
+  <autoFilter ref="A1:I24" xr:uid="{E5DF4185-7D09-482C-B551-D12CDF735AD0}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DC54D89C-B187-470B-A73E-9595AC905D54}" name="hidden_size"/>
     <tableColumn id="2" xr3:uid="{4865C0F4-76F1-4F26-A024-57E1FB83BD98}" name="batch_size"/>
     <tableColumn id="3" xr3:uid="{925130B2-7BA6-4EB7-954B-6B6B681EAB57}" name="learning_rate"/>
@@ -184,19 +366,7 @@
     <tableColumn id="6" xr3:uid="{05C7F77A-35FC-4154-B856-7B5788BECF81}" name="configuration"/>
     <tableColumn id="7" xr3:uid="{20D64F6D-6607-4B45-8B4E-114BF90DEACE}" name="HuberLoss 1st fold, test 1"/>
     <tableColumn id="8" xr3:uid="{7A22A143-39AD-432A-A231-3D5CE186C3F6}" name="HuberLoss 1st fold, test 2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BF0D451-C4EC-4C76-9533-946C338A61F1}" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{9BF0D451-C4EC-4C76-9533-946C338A61F1}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D6A26C0A-B170-414A-9726-CCF11976421E}" name="Benchmark"/>
-    <tableColumn id="2" xr3:uid="{015C6591-6245-40B5-BB2D-76513559F01D}" name="Huber"/>
-    <tableColumn id="3" xr3:uid="{2A4C1E94-F15F-48EB-9380-5F928EB498CE}" name="MAE / MW"/>
-    <tableColumn id="4" xr3:uid="{320F445D-AC0A-4F8E-B04F-0E25183BD0DB}" name="MSE /MW²"/>
+    <tableColumn id="9" xr3:uid="{304C15BB-8521-4AC0-9555-962BE52A200C}" name="HuberLoss 1st fold, test 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -519,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B619DEB1-2169-4C96-A144-21EC908D0785}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,9 +705,10 @@
     <col min="6" max="6" width="62.81640625" customWidth="1"/>
     <col min="7" max="7" width="18.1796875" customWidth="1"/>
     <col min="8" max="8" width="17.26953125" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,13 +728,16 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4</v>
       </c>
@@ -586,7 +760,7 @@
         <v>35.369999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>8</v>
       </c>
@@ -594,7 +768,7 @@
         <v>29.28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>16</v>
       </c>
@@ -602,7 +776,7 @@
         <v>27.01</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>32</v>
       </c>
@@ -610,7 +784,7 @@
         <v>24.75</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>64</v>
       </c>
@@ -618,7 +792,7 @@
         <v>23.94</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>128</v>
       </c>
@@ -626,7 +800,7 @@
         <v>23.86</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>256</v>
       </c>
@@ -634,7 +808,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -645,7 +819,7 @@
         <v>23.85</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>32</v>
       </c>
@@ -653,7 +827,7 @@
         <v>22.56</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>16</v>
       </c>
@@ -661,7 +835,7 @@
         <v>20.98</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>8</v>
       </c>
@@ -669,7 +843,7 @@
         <v>20.39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2">
         <v>4</v>
       </c>
@@ -677,7 +851,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -688,7 +862,7 @@
         <v>19.57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="1">
         <v>1E-4</v>
       </c>
@@ -696,7 +870,7 @@
         <v>24.63</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>32</v>
       </c>
@@ -713,7 +887,7 @@
         <v>22.25</v>
       </c>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F17" t="s">
         <v>10</v>
       </c>
@@ -721,15 +895,24 @@
         <v>37.64</v>
       </c>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F18" t="s">
         <v>11</v>
       </c>
       <c r="G18">
         <v>19.77</v>
       </c>
-    </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
@@ -739,25 +922,49 @@
       <c r="H19">
         <v>18.55</v>
       </c>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G20">
         <v>19.45</v>
       </c>
-    </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F21" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G21">
         <v>19.27</v>
       </c>
-    </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F22" t="s">
+      <c r="K21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="F22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G22">
@@ -767,23 +974,46 @@
         <v>18.43</v>
       </c>
     </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F23" t="s">
-        <v>18</v>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="F23" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="H23">
         <v>18.760000000000002</v>
       </c>
     </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F24" t="s">
-        <v>23</v>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="F24" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="H24">
         <v>18.38</v>
       </c>
     </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.35">
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -793,79 +1023,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89C0B56-1B29-407E-B99F-D49EFD255F23}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="53.453125" customWidth="1"/>
+    <col min="4" max="4" width="59.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>27.33</v>
-      </c>
-      <c r="C2">
-        <v>27.79</v>
-      </c>
-      <c r="D2">
-        <v>2986</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>25.53</v>
-      </c>
-      <c r="C3">
-        <v>25.99</v>
-      </c>
-      <c r="D3">
-        <v>2728.96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>28.01</v>
-      </c>
-      <c r="C4">
-        <v>28.48</v>
-      </c>
-      <c r="D4">
-        <v>3127.33</v>
+    <row r="1" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>